<commit_message>
file all converted, backup
</commit_message>
<xml_diff>
--- a/legislator/property/output/tmp6101_李鴻鈞_2011-11-17_財產申報表.xlsx
+++ b/legislator/property/output/tmp6101_李鴻鈞_2011-11-17_財產申報表.xlsx
@@ -9,13 +9,27 @@
   <sheets>
     <sheet name="土地" sheetId="1" r:id="rId1"/>
     <sheet name="建物" sheetId="2" r:id="rId2"/>
+    <sheet name="船舶" sheetId="3" r:id="rId3"/>
+    <sheet name="汽車" sheetId="4" r:id="rId4"/>
+    <sheet name="航空器" sheetId="5" r:id="rId5"/>
+    <sheet name="現金" sheetId="6" r:id="rId6"/>
+    <sheet name="存款" sheetId="7" r:id="rId7"/>
+    <sheet name="股票" sheetId="8" r:id="rId8"/>
+    <sheet name="債券" sheetId="9" r:id="rId9"/>
+    <sheet name="基金受益憑證" sheetId="10" r:id="rId10"/>
+    <sheet name="其他有價證券" sheetId="11" r:id="rId11"/>
+    <sheet name="具有相當價值之財產" sheetId="12" r:id="rId12"/>
+    <sheet name="保險" sheetId="13" r:id="rId13"/>
+    <sheet name="債權" sheetId="14" r:id="rId14"/>
+    <sheet name="債務" sheetId="15" r:id="rId15"/>
+    <sheet name="事業投資" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="166">
   <si>
     <t>土地坐落</t>
   </si>
@@ -210,6 +224,309 @@
   </si>
   <si>
     <t>1’870，000</t>
+  </si>
+  <si>
+    <t>種</t>
+  </si>
+  <si>
+    <t>類</t>
+  </si>
+  <si>
+    <t>總噸數</t>
+  </si>
+  <si>
+    <t>船籍港</t>
+  </si>
+  <si>
+    <t>所有人</t>
+  </si>
+  <si>
+    <t>廠牌型號</t>
+  </si>
+  <si>
+    <t>汽缸容量</t>
+  </si>
+  <si>
+    <t>•登記（取得）時間</t>
+  </si>
+  <si>
+    <t>BMW 740LI SEDAN</t>
+  </si>
+  <si>
+    <t>LEXUS ES350</t>
+  </si>
+  <si>
+    <t>劉素幸</t>
+  </si>
+  <si>
+    <t>96年02月 08日</t>
+  </si>
+  <si>
+    <t>97年04月 24 .日</t>
+  </si>
+  <si>
+    <t>型式</t>
+  </si>
+  <si>
+    <t>製造廠名稱</t>
+  </si>
+  <si>
+    <t>國籍標示及编號</t>
+  </si>
+  <si>
+    <t>幣別</t>
+  </si>
+  <si>
+    <t>.外幣總額</t>
+  </si>
+  <si>
+    <t>新臺幣總額或折合新臺幣總骄</t>
+  </si>
+  <si>
+    <t>存放梭構(應敘明分支機構）</t>
+  </si>
+  <si>
+    <t>種類</t>
+  </si>
+  <si>
+    <t>外幣總額</t>
+  </si>
+  <si>
+    <t>新臺幣總額或折合新臺幣總額</t>
+  </si>
+  <si>
+    <t>臺北縣泰山鄉農會</t>
+  </si>
+  <si>
+    <t>陽信商業銀行</t>
+  </si>
+  <si>
+    <t>中國信託商業銀行</t>
+  </si>
+  <si>
+    <t>合作金庫商業銀行</t>
+  </si>
+  <si>
+    <t>台灣銀行</t>
+  </si>
+  <si>
+    <t>第一商業銀行</t>
+  </si>
+  <si>
+    <t>臺灣土地銀行</t>
+  </si>
+  <si>
+    <t>國泰世華商業銀行</t>
+  </si>
+  <si>
+    <t>上海商業儲蓄銀行</t>
+  </si>
+  <si>
+    <t>中華郵政股份有限公司</t>
+  </si>
+  <si>
+    <t>國泰世華商業銀行敦化分 行</t>
+  </si>
+  <si>
+    <t>活期儲蓄存款</t>
+  </si>
+  <si>
+    <t>綜合存款</t>
+  </si>
+  <si>
+    <t>活期存款</t>
+  </si>
+  <si>
+    <t>新臺幣</t>
+  </si>
+  <si>
+    <t>新臺$</t>
+  </si>
+  <si>
+    <t>劉窣幸</t>
+  </si>
+  <si>
+    <t>名稱</t>
+  </si>
+  <si>
+    <t>股數</t>
+  </si>
+  <si>
+    <t>票面價額</t>
+  </si>
+  <si>
+    <t>外幣幣別</t>
+  </si>
+  <si>
+    <t>欣泰石油氣股份有限公司</t>
+  </si>
+  <si>
+    <t>晨星半導體股份有限公司</t>
+  </si>
+  <si>
+    <t>名</t>
+  </si>
+  <si>
+    <t>稱</t>
+  </si>
+  <si>
+    <t>代碼</t>
+  </si>
+  <si>
+    <t>買賣機構</t>
+  </si>
+  <si>
+    <t>單位數</t>
+  </si>
+  <si>
+    <t>受託投資機構</t>
+  </si>
+  <si>
+    <t>票面價額(單位淨值）</t>
+  </si>
+  <si>
+    <t>所</t>
+  </si>
+  <si>
+    <t>有</t>
+  </si>
+  <si>
+    <t>人</t>
+  </si>
+  <si>
+    <t>價</t>
+  </si>
+  <si>
+    <t>額</t>
+  </si>
+  <si>
+    <t>財產種類</t>
+  </si>
+  <si>
+    <t>項/</t>
+  </si>
+  <si>
+    <t>件</t>
+  </si>
+  <si>
+    <t>保險公司</t>
+  </si>
+  <si>
+    <t>保險名稱</t>
+  </si>
+  <si>
+    <t>要保人</t>
+  </si>
+  <si>
+    <t>備炷</t>
+  </si>
+  <si>
+    <t>安泰人壽</t>
+  </si>
+  <si>
+    <t>靈活理財變額保險乙型(投資 型保險）</t>
+  </si>
+  <si>
+    <t>靈活理財變額保險乙型(投資 型榇險）</t>
+  </si>
+  <si>
+    <t>債</t>
+  </si>
+  <si>
+    <t>權</t>
+  </si>
+  <si>
+    <t>債務人及地址</t>
+  </si>
+  <si>
+    <t>餘</t>
+  </si>
+  <si>
+    <t>取得（發生）時間</t>
+  </si>
+  <si>
+    <t>取得（發生）原因</t>
+  </si>
+  <si>
+    <t>債務人</t>
+  </si>
+  <si>
+    <t>債權人及地址</t>
+  </si>
+  <si>
+    <t>餘額</t>
+  </si>
+  <si>
+    <t>取得（發生)原因</t>
+  </si>
+  <si>
+    <t>抵押貸款</t>
+  </si>
+  <si>
+    <t>抵押貸款.</t>
+  </si>
+  <si>
+    <t>抵押貸款 .</t>
+  </si>
+  <si>
+    <t>陽信商業銀行 臺北市士林區中正路</t>
+  </si>
+  <si>
+    <t>第一商業銀行 臺北市中正區重慶南路</t>
+  </si>
+  <si>
+    <t>合庫商業銀行 臺北市中正區館前路</t>
+  </si>
+  <si>
+    <t>台灣土地銀行 臺北市中正區館前路</t>
+  </si>
+  <si>
+    <t>96年05月 16日</t>
+  </si>
+  <si>
+    <t>82年11月 09日</t>
+  </si>
+  <si>
+    <t>97年05月 13日</t>
+  </si>
+  <si>
+    <t>98年06月 19日</t>
+  </si>
+  <si>
+    <t>購屋貸款</t>
+  </si>
+  <si>
+    <t>購屋貸款，</t>
+  </si>
+  <si>
+    <t>購地融資</t>
+  </si>
+  <si>
+    <t>投資人</t>
+  </si>
+  <si>
+    <t>投資事業名稱</t>
+  </si>
+  <si>
+    <t>投資事業地址</t>
+  </si>
+  <si>
+    <t>投資金額</t>
+  </si>
+  <si>
+    <t>取得（發生）原.因</t>
+  </si>
+  <si>
+    <t>永錡加油站股份有限公司</t>
+  </si>
+  <si>
+    <t>新北市泰林路二段47號</t>
+  </si>
+  <si>
+    <t>86年01月 27日</t>
+  </si>
+  <si>
+    <t>原始股東</t>
   </si>
 </sst>
 </file>
@@ -940,6 +1257,472 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:8">
+      <c r="B1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:11">
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:7">
+      <c r="B1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
+        <v>123</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>124</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:K1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:11">
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>134</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="2">
+        <v>7793577</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>135</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="2">
+        <v>9800000</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>136</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="2">
+        <v>9800000</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>137</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="2">
+        <v>506059</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>138</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" s="2">
+        <v>9878940</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>140</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" s="2">
+        <v>15500000</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>141</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="2">
+        <v>49900000</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>146</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2000000</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J10"/>
@@ -1232,4 +2015,719 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:9">
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>58</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4000</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="2">
+        <v>4200000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>59</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3456</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2050000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:8">
+      <c r="B1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:5">
+      <c r="B1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>73</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2">
+        <v>1389320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>74</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2">
+        <v>3748061</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>75</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2">
+        <v>62120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="1">
+        <v>76</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2">
+        <v>220471</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="1">
+        <v>77</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
+        <v>2092079</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1">
+        <v>78</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2">
+        <v>4025</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1">
+        <v>79</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2">
+        <v>436526</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1">
+        <v>80</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2">
+        <v>1330726</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1">
+        <v>81</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <v>432939</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1">
+        <v>82</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1">
+        <v>83</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2">
+        <v>218467</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1">
+        <v>84</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2">
+        <v>308807</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1">
+        <v>85</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2">
+        <v>481934</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1">
+        <v>86</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="1">
+        <v>87</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2">
+        <v>11600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="1">
+        <v>88</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2">
+        <v>2270000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="1">
+        <v>89</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2">
+        <v>231830</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>96</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2">
+        <v>77854</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="2">
+        <v>778540</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>97</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="2">
+        <v>77335</v>
+      </c>
+      <c r="E3" s="2">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="2">
+        <v>773350</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1">
+        <v>98</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="2">
+        <v>25320</v>
+      </c>
+      <c r="E4" s="2">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="2">
+        <v>253200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:10">
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
issue #5: more cleaned data
</commit_message>
<xml_diff>
--- a/legislator/property/output/tmp6101_李鴻鈞_2011-11-17_財產申報表.xlsx
+++ b/legislator/property/output/tmp6101_李鴻鈞_2011-11-17_財產申報表.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="165">
   <si>
     <t>土地坐落</t>
   </si>
@@ -85,145 +85,142 @@
     <t>臺北市大安區通化段五小段 0425-0008 地號</t>
   </si>
   <si>
-    <t>土 地坐落</t>
+    <t>10000分之 59</t>
+  </si>
+  <si>
+    <t>10000分之 129</t>
+  </si>
+  <si>
+    <t>10000分之 252</t>
+  </si>
+  <si>
+    <t>10000分之 89</t>
+  </si>
+  <si>
+    <t>10000分之 105</t>
+  </si>
+  <si>
+    <t>100000 分 之226</t>
+  </si>
+  <si>
+    <t>10分之1</t>
+  </si>
+  <si>
+    <t>李鴻鈞</t>
+  </si>
+  <si>
+    <t>李鴻韵</t>
+  </si>
+  <si>
+    <t>89年07月 24日</t>
+  </si>
+  <si>
+    <t>82年05月 26日</t>
+  </si>
+  <si>
+    <t>82年Q5月 26日</t>
+  </si>
+  <si>
+    <t>96年04月 17日</t>
+  </si>
+  <si>
+    <t>97年02月 12日</t>
+  </si>
+  <si>
+    <t>98年02月 03日</t>
+  </si>
+  <si>
+    <t>98年05月 22日</t>
+  </si>
+  <si>
+    <t>買賣</t>
+  </si>
+  <si>
+    <t>貝賈</t>
+  </si>
+  <si>
+    <t>貝賣</t>
+  </si>
+  <si>
+    <t>(超過五年）</t>
+  </si>
+  <si>
+    <t>(超過五年)’</t>
+  </si>
+  <si>
+    <t>50，565，900</t>
+  </si>
+  <si>
+    <t>1，207，500</t>
+  </si>
+  <si>
+    <t>建物標示</t>
+  </si>
+  <si>
+    <t>臺北市中正區中正段二小段 01938-000 建號（（陽台 10.5$ 平 方公尺花台4.78平方公尺））</t>
+  </si>
+  <si>
+    <t>臺北市中正區中正段二小段 01928-000 建號</t>
+  </si>
+  <si>
+    <t>新北市泰山區黎明段00621-000 建號((陽台13.44平方公尺花台 0.70平方公尺））</t>
+  </si>
+  <si>
+    <t>新北市泰山區同興段04004-000 建號((含停車位編號104號))</t>
+  </si>
+  <si>
+    <t>新北市泰山區同興段04017-000 建號((含停車位編號103號））.</t>
+  </si>
+  <si>
+    <t>新北市泰山區同興段04001-000 建號((含停車位編號128號及陽 台7.94平方公尺））</t>
+  </si>
+  <si>
+    <t>新北市泰山區同興段04014-000 建號（（含停車位編號129號及陽 台10.03平方公尺））</t>
+  </si>
+  <si>
+    <t>新北市淡水區海天段02913-000 建號((含停車位2位編號41.42 號））</t>
+  </si>
+  <si>
+    <t>建 物</t>
+  </si>
+  <si>
+    <t>標</t>
+  </si>
+  <si>
+    <t>全部</t>
+  </si>
+  <si>
+    <t>56分之1</t>
+  </si>
+  <si>
+    <t>示</t>
+  </si>
+  <si>
+    <t>李鴻鈞 ■</t>
   </si>
   <si>
     <t>面積（平方 公尺）</t>
   </si>
   <si>
-    <t>10000分之 59</t>
-  </si>
-  <si>
-    <t>10000分之 129</t>
-  </si>
-  <si>
-    <t>10000分之 252</t>
-  </si>
-  <si>
-    <t>10000分之 89</t>
-  </si>
-  <si>
-    <t>10000分之 105</t>
-  </si>
-  <si>
-    <t>100000 分 之226</t>
-  </si>
-  <si>
-    <t>10分之1</t>
+    <t>98年02月 04日</t>
   </si>
   <si>
     <t>權利範圍 (持分）</t>
   </si>
   <si>
-    <t>李鴻鈞</t>
-  </si>
-  <si>
-    <t>李鴻韵</t>
-  </si>
-  <si>
-    <t>89年07月 24日</t>
-  </si>
-  <si>
-    <t>82年05月 26日</t>
-  </si>
-  <si>
-    <t>82年Q5月 26日</t>
-  </si>
-  <si>
-    <t>96年04月 17日</t>
-  </si>
-  <si>
-    <t>97年02月 12日</t>
-  </si>
-  <si>
-    <t>98年02月 03日</t>
-  </si>
-  <si>
-    <t>98年05月 22日</t>
+    <t>3’680，000</t>
+  </si>
+  <si>
+    <t>1’870，000</t>
   </si>
   <si>
     <t>變動時間</t>
   </si>
   <si>
-    <t>買賣</t>
-  </si>
-  <si>
-    <t>貝賈</t>
-  </si>
-  <si>
-    <t>貝賣</t>
-  </si>
-  <si>
     <t>變動原因</t>
   </si>
   <si>
-    <t>(超過五年）</t>
-  </si>
-  <si>
-    <t>(超過五年)’</t>
-  </si>
-  <si>
-    <t>50，565，900</t>
-  </si>
-  <si>
-    <t>1，207，500</t>
-  </si>
-  <si>
     <t>變動時之價額</t>
-  </si>
-  <si>
-    <t>建物標示</t>
-  </si>
-  <si>
-    <t>臺北市中正區中正段二小段 01938-000 建號（（陽台 10.5$ 平 方公尺花台4.78平方公尺））</t>
-  </si>
-  <si>
-    <t>臺北市中正區中正段二小段 01928-000 建號</t>
-  </si>
-  <si>
-    <t>新北市泰山區黎明段00621-000 建號((陽台13.44平方公尺花台 0.70平方公尺））</t>
-  </si>
-  <si>
-    <t>新北市泰山區同興段04004-000 建號((含停車位編號104號))</t>
-  </si>
-  <si>
-    <t>新北市泰山區同興段04017-000 建號((含停車位編號103號））.</t>
-  </si>
-  <si>
-    <t>新北市泰山區同興段04001-000 建號((含停車位編號128號及陽 台7.94平方公尺））</t>
-  </si>
-  <si>
-    <t>新北市泰山區同興段04014-000 建號（（含停車位編號129號及陽 台10.03平方公尺））</t>
-  </si>
-  <si>
-    <t>新北市淡水區海天段02913-000 建號((含停車位2位編號41.42 號））</t>
-  </si>
-  <si>
-    <t>建 物</t>
-  </si>
-  <si>
-    <t>標</t>
-  </si>
-  <si>
-    <t>全部</t>
-  </si>
-  <si>
-    <t>56分之1</t>
-  </si>
-  <si>
-    <t>示</t>
-  </si>
-  <si>
-    <t>李鴻鈞 ■</t>
-  </si>
-  <si>
-    <t>98年02月 04日</t>
-  </si>
-  <si>
-    <t>3’680，000</t>
-  </si>
-  <si>
-    <t>1’870，000</t>
   </si>
   <si>
     <t>種</t>
@@ -885,7 +882,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -925,19 +922,19 @@
         <v>2023</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -951,19 +948,19 @@
         <v>402</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -977,19 +974,19 @@
         <v>87</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1003,19 +1000,19 @@
         <v>1904.77</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1029,19 +1026,19 @@
         <v>21.21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1055,19 +1052,19 @@
         <v>22.2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1081,16 +1078,16 @@
         <v>4863.81</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H8" s="2">
         <v>16960000</v>
@@ -1107,16 +1104,16 @@
         <v>4863.81</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="H9" s="2">
         <v>9390000</v>
@@ -1133,16 +1130,16 @@
         <v>13558.99</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H10" s="2">
         <v>11520000</v>
@@ -1159,19 +1156,19 @@
         <v>796</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -1185,19 +1182,19 @@
         <v>19</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1211,45 +1208,19 @@
         <v>168</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H13" s="2">
         <v>10672200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="1">
-        <v>29</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1267,25 +1238,25 @@
   <sheetData>
     <row r="1" spans="2:8">
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1303,34 +1274,34 @@
   <sheetData>
     <row r="1" spans="2:11">
       <c r="B1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1348,22 +1319,22 @@
   <sheetData>
     <row r="1" spans="2:7">
       <c r="B1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1381,16 +1352,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1398,13 +1369,13 @@
         <v>123</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>131</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -1413,13 +1384,13 @@
         <v>124</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -1438,34 +1409,34 @@
   <sheetData>
     <row r="1" spans="2:11">
       <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1483,22 +1454,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1506,22 +1477,22 @@
         <v>134</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E2" s="2">
         <v>7793577</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1529,22 +1500,22 @@
         <v>135</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E3" s="2">
         <v>9800000</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1552,22 +1523,22 @@
         <v>136</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E4" s="2">
         <v>9800000</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1575,22 +1546,22 @@
         <v>137</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E5" s="2">
         <v>506059</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1598,22 +1569,22 @@
         <v>138</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E6" s="2">
         <v>9878940</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1621,22 +1592,22 @@
         <v>140</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E7" s="2">
         <v>15500000</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1644,22 +1615,22 @@
         <v>141</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E8" s="2">
         <v>49900000</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1677,22 +1648,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1700,22 +1671,22 @@
         <v>146</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="E2" s="2">
         <v>2000000</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1733,7 +1704,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1761,25 +1732,25 @@
         <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2">
         <v>87.2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -1789,25 +1760,25 @@
         <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2">
         <v>2132.23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1817,25 +1788,25 @@
         <v>39</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2">
         <v>102.19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1845,22 +1816,22 @@
         <v>40</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2">
         <v>75.84</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H5" s="2">
         <v>3570000</v>
@@ -1873,25 +1844,25 @@
         <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2">
         <v>77.52</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1901,22 +1872,22 @@
         <v>42</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C7" s="2">
         <v>92.66</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="H7" s="2">
         <v>2160000</v>
@@ -1929,25 +1900,25 @@
         <v>43</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C8" s="2">
         <v>77.61</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="H8" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1957,22 +1928,22 @@
         <v>44</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C9" s="2">
         <v>145.47</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H9" s="2">
         <v>10480000</v>
@@ -1985,31 +1956,31 @@
         <v>47</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="F10" s="2" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2027,19 +1998,19 @@
   <sheetData>
     <row r="1" spans="2:9">
       <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -2066,16 +2037,16 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -2089,19 +2060,19 @@
         <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="2">
         <v>4000</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G2" s="2">
         <v>4200000</v>
@@ -2112,19 +2083,19 @@
         <v>59</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="2">
         <v>3456</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G3" s="2">
         <v>2050000</v>
@@ -2145,16 +2116,16 @@
   <sheetData>
     <row r="1" spans="2:8">
       <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>80</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -2181,16 +2152,16 @@
   <sheetData>
     <row r="1" spans="2:5">
       <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -2208,22 +2179,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2231,16 +2202,16 @@
         <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2">
@@ -2252,16 +2223,16 @@
         <v>74</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
@@ -2273,16 +2244,16 @@
         <v>75</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
@@ -2294,16 +2265,16 @@
         <v>76</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
@@ -2315,16 +2286,16 @@
         <v>77</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
@@ -2336,16 +2307,16 @@
         <v>78</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2">
@@ -2357,16 +2328,16 @@
         <v>79</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
@@ -2378,16 +2349,16 @@
         <v>80</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
@@ -2399,16 +2370,16 @@
         <v>81</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
@@ -2420,16 +2391,16 @@
         <v>82</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2">
@@ -2441,16 +2412,16 @@
         <v>83</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2">
@@ -2462,16 +2433,16 @@
         <v>84</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
@@ -2483,16 +2454,16 @@
         <v>85</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2">
@@ -2504,16 +2475,16 @@
         <v>86</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2">
@@ -2525,16 +2496,16 @@
         <v>87</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2">
@@ -2546,16 +2517,16 @@
         <v>88</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2">
@@ -2567,16 +2538,16 @@
         <v>89</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2">
@@ -2598,22 +2569,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2621,10 +2592,10 @@
         <v>96</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2">
         <v>77854</v>
@@ -2633,7 +2604,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G2" s="2">
         <v>778540</v>
@@ -2644,10 +2615,10 @@
         <v>97</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2">
         <v>77335</v>
@@ -2656,7 +2627,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G3" s="2">
         <v>773350</v>
@@ -2667,10 +2638,10 @@
         <v>98</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" s="2">
         <v>25320</v>
@@ -2679,7 +2650,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G4" s="2">
         <v>253200</v>
@@ -2700,31 +2671,31 @@
   <sheetData>
     <row r="1" spans="2:10">
       <c r="B1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="H1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>